<commit_message>
add OFRA to 2023 spp comparisons, combine N+S Palm Beach Subregions
</commit_message>
<xml_diff>
--- a/data/species_metadata.xlsx
+++ b/data/species_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcunning/Projects/DRM2024/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosscunning/Projects/DRM2024/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5E1A96-B914-7D40-B2ED-6B2191D6AF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53833CF0-A705-4549-B941-01F96F351CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{D5AFB406-C22B-2F4F-AAB8-07025DABA21B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
   <si>
     <t>Species</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t xml:space="preserve">MYCE </t>
+  </si>
+  <si>
+    <t>OFRA</t>
   </si>
 </sst>
 </file>
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610B4843-1A22-CE44-BF5C-49505C673594}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1122,6 +1125,23 @@
         <v>39</v>
       </c>
     </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>